<commit_message>
Added packages in project
</commit_message>
<xml_diff>
--- a/Daily updates.xlsx
+++ b/Daily updates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Wipro\Capstone Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{591AF97E-D999-44E1-AE86-A56279B9895E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F2D4D2C-2A29-45F4-9956-FBE1D49E2ACA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1B68D35D-05E9-44FA-896A-31A412F72FAE}"/>
   </bookViews>
@@ -82,7 +82,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,6 +103,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -125,11 +131,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,8 +453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F181682F-695A-4C4E-8848-15D387841887}">
   <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -482,7 +489,7 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -491,13 +498,13 @@
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="4" t="s">
         <v>9</v>
       </c>
       <c r="L1" s="1" t="s">
@@ -506,10 +513,10 @@
       <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="4" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>